<commit_message>
Set intro activity to make splash screen. Animation is set up.
</commit_message>
<xml_diff>
--- a/Additional Files/Processing/Processing Sheet.xlsx
+++ b/Additional Files/Processing/Processing Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\Project\Android_Project\SSLC\Additional Files\Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65C5BD0-14B5-4023-8CFB-39E1A3960456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F960B22-974B-4E1C-AB64-8B6A013686BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A62076EC-93F2-4166-BAB8-D05A3EE4D5F4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Number</t>
   </si>
@@ -55,13 +55,29 @@
     <t>IntroActivity</t>
   </si>
   <si>
-    <t>Show Logo for 2 secs then go to main</t>
-  </si>
-  <si>
     <t>How to</t>
   </si>
   <si>
     <t>Mar 16, 2022</t>
+  </si>
+  <si>
+    <t>Show Logo for 3 secs then move to Login Activity</t>
+  </si>
+  <si>
+    <t>1. Create Animation Resoure File.
+2. Create Imageview in Layout.
+3. Set the animation in IntroLayout.
+4. Connect animation to ImageView.</t>
+  </si>
+  <si>
+    <t>Main : 
+IntroActivity
+LoginActivity
+Resources : 
+side_slide.xml
+ic_logo.gif
+activity_intro.xml
+activity_login.xml</t>
   </si>
 </sst>
 </file>
@@ -94,7 +110,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +120,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,15 +157,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,58 +497,67 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="23.4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="129.6">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
+      <c r="F3" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>